<commit_message>
Last field day of 2024
</commit_message>
<xml_diff>
--- a/Field_Days.xlsx
+++ b/Field_Days.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jacob/Desktop/Projects/Field-Days/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D0B6476D-B1BD-8F4B-85D8-7F2E9D5DAD04}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{508F78F9-DC5E-D348-A73C-B15A288C841C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15960" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -574,7 +574,6 @@
       <b/>
       <sz val="12"/>
       <name val="Calibri"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="5">
@@ -1111,7 +1110,7 @@
           </c:val>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-22E0-0643-927F-2498D3EB4157}"/>
+              <c16:uniqueId val="{00000000-B943-3942-A2A1-54A971CC8D6E}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -1216,7 +1215,7 @@
           </c:val>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000001-22E0-0643-927F-2498D3EB4157}"/>
+              <c16:uniqueId val="{00000001-B943-3942-A2A1-54A971CC8D6E}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -1321,7 +1320,7 @@
           </c:val>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000002-22E0-0643-927F-2498D3EB4157}"/>
+              <c16:uniqueId val="{00000002-B943-3942-A2A1-54A971CC8D6E}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -1426,7 +1425,7 @@
           </c:val>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000003-22E0-0643-927F-2498D3EB4157}"/>
+              <c16:uniqueId val="{00000003-B943-3942-A2A1-54A971CC8D6E}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -1531,7 +1530,7 @@
           </c:val>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000004-22E0-0643-927F-2498D3EB4157}"/>
+              <c16:uniqueId val="{00000004-B943-3942-A2A1-54A971CC8D6E}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -1636,7 +1635,7 @@
           </c:val>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000005-22E0-0643-927F-2498D3EB4157}"/>
+              <c16:uniqueId val="{00000005-B943-3942-A2A1-54A971CC8D6E}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -1743,7 +1742,7 @@
           </c:val>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000006-22E0-0643-927F-2498D3EB4157}"/>
+              <c16:uniqueId val="{00000006-B943-3942-A2A1-54A971CC8D6E}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -1838,7 +1837,7 @@
           </c:val>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000007-22E0-0643-927F-2498D3EB4157}"/>
+              <c16:uniqueId val="{00000007-B943-3942-A2A1-54A971CC8D6E}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -2390,7 +2389,7 @@
           </c:val>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-CA36-0646-BE7E-2B259DC0BDD8}"/>
+              <c16:uniqueId val="{00000000-2402-604F-B454-3801CEF99BBF}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -2495,7 +2494,7 @@
           </c:val>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000001-CA36-0646-BE7E-2B259DC0BDD8}"/>
+              <c16:uniqueId val="{00000001-2402-604F-B454-3801CEF99BBF}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -2600,7 +2599,7 @@
           </c:val>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000002-CA36-0646-BE7E-2B259DC0BDD8}"/>
+              <c16:uniqueId val="{00000002-2402-604F-B454-3801CEF99BBF}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -2705,7 +2704,7 @@
           </c:val>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000003-CA36-0646-BE7E-2B259DC0BDD8}"/>
+              <c16:uniqueId val="{00000003-2402-604F-B454-3801CEF99BBF}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -2810,7 +2809,7 @@
           </c:val>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000004-CA36-0646-BE7E-2B259DC0BDD8}"/>
+              <c16:uniqueId val="{00000004-2402-604F-B454-3801CEF99BBF}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -2915,7 +2914,7 @@
           </c:val>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000005-CA36-0646-BE7E-2B259DC0BDD8}"/>
+              <c16:uniqueId val="{00000005-2402-604F-B454-3801CEF99BBF}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -3022,7 +3021,7 @@
           </c:val>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000006-CA36-0646-BE7E-2B259DC0BDD8}"/>
+              <c16:uniqueId val="{00000006-2402-604F-B454-3801CEF99BBF}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -3117,7 +3116,7 @@
           </c:val>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000007-CA36-0646-BE7E-2B259DC0BDD8}"/>
+              <c16:uniqueId val="{00000007-2402-604F-B454-3801CEF99BBF}"/>
             </c:ext>
           </c:extLst>
         </c:ser>

</xml_diff>